<commit_message>
added Facebook post reading and Managers screen
</commit_message>
<xml_diff>
--- a/GenXServiceEngagementCenterApplication/AnalyticalReports/Tickets based on Priority.xlsx
+++ b/GenXServiceEngagementCenterApplication/AnalyticalReports/Tickets based on Priority.xlsx
@@ -12,7 +12,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="107" uniqueCount="43">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="122" uniqueCount="47">
   <si>
     <t>CHANNELID</t>
   </si>
@@ -35,48 +35,48 @@
     <t>STATUS</t>
   </si>
   <si>
+    <t>FACEBOOK</t>
+  </si>
+  <si>
+    <t>OneNote</t>
+  </si>
+  <si>
+    <t>Microsoft OneNote ended with an error is taking too long to open</t>
+  </si>
+  <si>
+    <t>HIGH</t>
+  </si>
+  <si>
+    <t>CLOSED</t>
+  </si>
+  <si>
+    <t>Excel</t>
+  </si>
+  <si>
+    <t>Microsoft Excel ended with an error is not able to open charts</t>
+  </si>
+  <si>
     <t>APPLICATION</t>
   </si>
   <si>
-    <t>OneNote</t>
+    <t>PictureMgr</t>
+  </si>
+  <si>
+    <t>Microsoft PictureMgr ended with an error not able to start</t>
+  </si>
+  <si>
+    <t>Access</t>
+  </si>
+  <si>
+    <t>Microsoft Access ended with an error is not able to open charts</t>
   </si>
   <si>
     <t>Microsoft OneNote ended with an error is not able to connect to API</t>
   </si>
   <si>
-    <t>HIGH</t>
-  </si>
-  <si>
-    <t>CLOSED</t>
-  </si>
-  <si>
-    <t>FACEBOOK</t>
-  </si>
-  <si>
-    <t>Microsoft OneNote ended with an error is taking too long to open</t>
-  </si>
-  <si>
-    <t>PictureMgr</t>
-  </si>
-  <si>
-    <t>Microsoft PictureMgr ended with an error not able to start</t>
-  </si>
-  <si>
-    <t>Excel</t>
-  </si>
-  <si>
     <t>Microsoft Excel ended with an error is hanging</t>
   </si>
   <si>
-    <t>Microsoft Excel ended with an error is not able to open charts</t>
-  </si>
-  <si>
-    <t>Access</t>
-  </si>
-  <si>
-    <t>Microsoft Access ended with an error is not able to open charts</t>
-  </si>
-  <si>
     <t>TWITTER</t>
   </si>
   <si>
@@ -116,28 +116,40 @@
     <t>Microsoft OneDrive ended with an error is taking too long to open</t>
   </si>
   <si>
+    <t>Publisher</t>
+  </si>
+  <si>
+    <t>Microsoft Publisher ended with an error is not able to start</t>
+  </si>
+  <si>
+    <t>MEDIUM</t>
+  </si>
+  <si>
+    <t>Ishan is now facing issues with Access</t>
+  </si>
+  <si>
+    <t>OPEN</t>
+  </si>
+  <si>
+    <t>Ishan is not able to run Microsoft Excel</t>
+  </si>
+  <si>
     <t>Project</t>
   </si>
   <si>
     <t>Microsoft Project ended with an error is not able to connect to API</t>
   </si>
   <si>
-    <t>MEDIUM</t>
-  </si>
-  <si>
     <t>Microsoft OneNote ended with an error is not able to start</t>
   </si>
   <si>
-    <t>Publisher</t>
-  </si>
-  <si>
-    <t>Microsoft Publisher ended with an error is not able to start</t>
-  </si>
-  <si>
     <t>Skype</t>
   </si>
   <si>
     <t>Microsoft Skype ended with an error is not able to connect to API</t>
+  </si>
+  <si>
+    <t>Hi I am not able to open Excel</t>
   </si>
   <si>
     <t>Microsoft OneNote ended with an error not able to start</t>
@@ -219,16 +231,16 @@
         <v>300.0</v>
       </c>
       <c r="B2" t="s">
-        <v>7</v>
+        <v>14</v>
       </c>
       <c r="C2" t="n">
-        <v>5.0</v>
+        <v>14.0</v>
       </c>
       <c r="D2" t="s">
-        <v>8</v>
+        <v>29</v>
       </c>
       <c r="E2" t="s">
-        <v>42</v>
+        <v>30</v>
       </c>
       <c r="F2" t="s">
         <v>36</v>

</xml_diff>